<commit_message>
Got restricted pi 2-eq results
</commit_message>
<xml_diff>
--- a/results/tables/final_tables_7_21.xlsx
+++ b/results/tables/final_tables_7_21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox (Boston University)\1_boston_university\8-Research Assistantship\ukData\results\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3922474-3ACD-4B39-99E4-E0F8078D684A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DBCA2E-428B-44A2-85B3-3077A18606AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" firstSheet="9" activeTab="13" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="656" firstSheet="7" activeTab="9" xr2:uid="{E382401A-5014-4F77-A3DB-04E9551C20F1}"/>
   </bookViews>
   <sheets>
     <sheet name="education_classification" sheetId="15" r:id="rId1"/>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="297">
   <si>
     <t>Occupation fixed-effects</t>
   </si>
@@ -1341,7 +1341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1503,6 +1503,7 @@
     <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="11" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2141,7 +2142,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2152,14 +2153,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="86" t="s">
         <v>276</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
     </row>
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="10"/>
@@ -2261,14 +2262,14 @@
     </row>
     <row r="8" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="85" t="s">
+      <c r="A9" s="86" t="s">
         <v>277</v>
       </c>
-      <c r="B9" s="85"/>
-      <c r="C9" s="85"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
+      <c r="B9" s="86"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
     </row>
     <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="10"/>
@@ -2386,8 +2387,8 @@
   </sheetPr>
   <dimension ref="A1:O62"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A9" zoomScale="90" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2397,20 +2398,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G2" s="85" t="s">
+      <c r="G2" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
     </row>
     <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
@@ -2437,18 +2438,10 @@
       <c r="I3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="80">
-        <v>2.3825693796604801E-2</v>
-      </c>
-      <c r="L3" s="80">
-        <v>8.6462761603051996E-2</v>
-      </c>
-      <c r="M3" s="80">
-        <v>9.1086936740078506E-2</v>
-      </c>
-      <c r="N3" s="80">
-        <v>9.1114556856590104E-2</v>
-      </c>
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="80"/>
+      <c r="N3" s="80"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -2478,35 +2471,27 @@
         <f t="shared" si="0"/>
         <v>1.0266230598457746</v>
       </c>
-      <c r="K4" s="80">
-        <v>2.3825693796604801E-2</v>
-      </c>
-      <c r="L4" s="80">
-        <v>0.102623074984331</v>
-      </c>
-      <c r="M4" s="80">
-        <v>9.9970167180033806E-2</v>
-      </c>
-      <c r="N4" s="80">
-        <v>0.131180946644253</v>
-      </c>
+      <c r="K4" s="80"/>
+      <c r="L4" s="80"/>
+      <c r="M4" s="80"/>
+      <c r="N4" s="80"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B5" s="73">
-        <f>+K7</f>
-        <v>-2.3825693796604801E-2</v>
-      </c>
-      <c r="C5" s="73">
-        <f t="shared" ref="C5:E5" si="1">+L7</f>
-        <v>-8.6462761603051996E-2</v>
-      </c>
-      <c r="D5" s="73">
+      <c r="B5" s="73" t="str">
+        <f>+IF(K7=0,"",K7)</f>
+        <v/>
+      </c>
+      <c r="C5" s="73" t="str">
+        <f t="shared" ref="C5:E5" si="1">+IF(L7=0,"",L7)</f>
+        <v/>
+      </c>
+      <c r="D5" s="73" t="str">
         <f t="shared" si="1"/>
-        <v>-9.1086936740078506E-2</v>
-      </c>
-      <c r="E5" s="73">
+        <v/>
+      </c>
+      <c r="E5" s="73" t="str">
         <f t="shared" si="1"/>
-        <v>-9.1114556856590104E-2</v>
+        <v/>
       </c>
       <c r="G5" s="18">
         <f>+C6/$B6</f>
@@ -2520,18 +2505,10 @@
         <f>+E6/$B6</f>
         <v>0.13736843489130302</v>
       </c>
-      <c r="K5" s="80">
-        <v>2.3825693796604801E-2</v>
-      </c>
-      <c r="L5" s="80">
-        <v>8.7913295104061095E-2</v>
-      </c>
-      <c r="M5" s="80">
-        <v>9.5241393813421102E-2</v>
-      </c>
-      <c r="N5" s="80">
-        <v>7.0074395414781599E-3</v>
-      </c>
+      <c r="K5" s="80"/>
+      <c r="L5" s="80"/>
+      <c r="M5" s="80"/>
+      <c r="N5" s="80"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -2563,37 +2540,37 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B7" s="73">
-        <f>+K8</f>
-        <v>-2.3825693796604801E-2</v>
-      </c>
-      <c r="C7" s="73">
-        <f t="shared" ref="C7:E7" si="2">+L8</f>
-        <v>-0.102623074984331</v>
-      </c>
-      <c r="D7" s="73">
+      <c r="B7" s="73" t="str">
+        <f>+IF(K8=0,"",K8)</f>
+        <v/>
+      </c>
+      <c r="C7" s="73" t="str">
+        <f t="shared" ref="C7:E7" si="2">+IF(L8=0,"",L8)</f>
+        <v/>
+      </c>
+      <c r="D7" s="73" t="str">
         <f t="shared" si="2"/>
-        <v>-9.9970167180033806E-2</v>
-      </c>
-      <c r="E7" s="73">
+        <v/>
+      </c>
+      <c r="E7" s="73" t="str">
         <f t="shared" si="2"/>
-        <v>-0.131180946644253</v>
+        <v/>
       </c>
       <c r="K7" s="80">
         <f>-K3</f>
-        <v>-2.3825693796604801E-2</v>
+        <v>0</v>
       </c>
       <c r="L7" s="80">
         <f t="shared" ref="L7:N7" si="3">-L3</f>
-        <v>-8.6462761603051996E-2</v>
+        <v>0</v>
       </c>
       <c r="M7" s="80">
         <f t="shared" si="3"/>
-        <v>-9.1086936740078506E-2</v>
+        <v>0</v>
       </c>
       <c r="N7" s="80">
         <f t="shared" si="3"/>
-        <v>-9.1114556856590104E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -2626,38 +2603,38 @@
       </c>
       <c r="K8" s="80">
         <f t="shared" ref="K8:N8" si="4">-K4</f>
-        <v>-2.3825693796604801E-2</v>
+        <v>0</v>
       </c>
       <c r="L8" s="80">
         <f t="shared" si="4"/>
-        <v>-0.102623074984331</v>
+        <v>0</v>
       </c>
       <c r="M8" s="80">
         <f t="shared" si="4"/>
-        <v>-9.9970167180033806E-2</v>
+        <v>0</v>
       </c>
       <c r="N8" s="80">
         <f t="shared" si="4"/>
-        <v>-0.131180946644253</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="19"/>
-      <c r="B9" s="74">
-        <f>+K9</f>
-        <v>-2.3825693796604801E-2</v>
-      </c>
-      <c r="C9" s="74">
-        <f t="shared" ref="C9:E9" si="5">+L9</f>
-        <v>-8.7913295104061095E-2</v>
-      </c>
-      <c r="D9" s="74">
+      <c r="B9" s="74" t="str">
+        <f>+IF(K9=0,"",K9)</f>
+        <v/>
+      </c>
+      <c r="C9" s="74" t="str">
+        <f t="shared" ref="C9:E9" si="5">+IF(L9=0,"",L9)</f>
+        <v/>
+      </c>
+      <c r="D9" s="74" t="str">
         <f t="shared" si="5"/>
-        <v>-9.5241393813421102E-2</v>
-      </c>
-      <c r="E9" s="74">
+        <v/>
+      </c>
+      <c r="E9" s="74" t="str">
         <f t="shared" si="5"/>
-        <v>-7.0074395414781599E-3</v>
+        <v/>
       </c>
       <c r="G9" s="80">
         <v>0.250506013088374</v>
@@ -2673,19 +2650,19 @@
       </c>
       <c r="K9" s="80">
         <f t="shared" ref="K9:N9" si="6">-K5</f>
-        <v>-2.3825693796604801E-2</v>
+        <v>0</v>
       </c>
       <c r="L9" s="80">
         <f t="shared" si="6"/>
-        <v>-8.7913295104061095E-2</v>
+        <v>0</v>
       </c>
       <c r="M9" s="80">
         <f t="shared" si="6"/>
-        <v>-9.5241393813421102E-2</v>
+        <v>0</v>
       </c>
       <c r="N9" s="80">
         <f t="shared" si="6"/>
-        <v>-7.0074395414781599E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -2737,11 +2714,11 @@
       <c r="B13" s="54">
         <v>62</v>
       </c>
-      <c r="G13" s="85" t="s">
+      <c r="G13" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="85"/>
-      <c r="I13" s="85"/>
+      <c r="H13" s="86"/>
+      <c r="I13" s="86"/>
       <c r="M13" s="81"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
@@ -2756,13 +2733,13 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="99" t="s">
+      <c r="A15" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="99"/>
-      <c r="C15" s="99"/>
-      <c r="D15" s="99"/>
-      <c r="E15" s="99"/>
+      <c r="B15" s="100"/>
+      <c r="C15" s="100"/>
+      <c r="D15" s="100"/>
+      <c r="E15" s="100"/>
       <c r="G15" s="18">
         <f t="shared" ref="G15:I17" si="7">+C18/$B18</f>
         <v>2.2692799840412765</v>
@@ -2906,11 +2883,11 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="G24" s="85" t="s">
+      <c r="G24" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="H24" s="85"/>
-      <c r="I24" s="85"/>
+      <c r="H24" s="86"/>
+      <c r="I24" s="86"/>
     </row>
     <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="G25" s="8" t="s">
@@ -2936,13 +2913,13 @@
       </c>
     </row>
     <row r="26" spans="1:15" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="99" t="s">
+      <c r="A26" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="99"/>
-      <c r="C26" s="99"/>
-      <c r="D26" s="99"/>
-      <c r="E26" s="99"/>
+      <c r="B26" s="100"/>
+      <c r="C26" s="100"/>
+      <c r="D26" s="100"/>
+      <c r="E26" s="100"/>
       <c r="G26" s="18">
         <f t="shared" ref="G26:I28" si="8">+C29/$B29</f>
         <v>1.0840988998256753</v>
@@ -3119,20 +3096,20 @@
       <c r="E36" s="1"/>
     </row>
     <row r="37" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="99" t="s">
+      <c r="A37" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="99"/>
-      <c r="C37" s="99"/>
-      <c r="D37" s="99"/>
-      <c r="E37" s="99"/>
+      <c r="B37" s="100"/>
+      <c r="C37" s="100"/>
+      <c r="D37" s="100"/>
+      <c r="E37" s="100"/>
     </row>
     <row r="38" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G38" s="85" t="s">
+      <c r="G38" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="H38" s="85"/>
-      <c r="I38" s="85"/>
+      <c r="H38" s="86"/>
+      <c r="I38" s="86"/>
     </row>
     <row r="39" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="10" t="s">
@@ -3160,149 +3137,133 @@
       <c r="I39" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="K39" s="80">
-        <v>1.8856321828307002E-2</v>
-      </c>
-      <c r="L39" s="80">
-        <v>7.4986834877180303E-2</v>
-      </c>
-      <c r="M39" s="80">
-        <v>0.114521497868232</v>
-      </c>
-      <c r="N39" s="80">
-        <v>0.14262511117377299</v>
-      </c>
+      <c r="K39" s="80"/>
+      <c r="L39" s="80"/>
+      <c r="M39" s="80"/>
+      <c r="N39" s="80"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>93</v>
       </c>
       <c r="B40" s="72">
-        <v>0.30002408033317401</v>
+        <f>+G45</f>
+        <v>0.26143821264262401</v>
       </c>
       <c r="C40" s="72">
-        <v>0.38983157888076198</v>
+        <f t="shared" ref="C40:E40" si="9">+H45</f>
+        <v>0.37164357323102198</v>
       </c>
       <c r="D40" s="72">
-        <v>0.77387006959986604</v>
+        <f t="shared" si="9"/>
+        <v>0.89501900335057205</v>
       </c>
       <c r="E40" s="72">
-        <v>0.132595645940602</v>
+        <f t="shared" si="9"/>
+        <v>4.5401966924630999E-2</v>
       </c>
       <c r="G40" s="18">
         <f>+C40/$B40</f>
-        <v>1.2993343015929173</v>
+        <v>1.421535013854476</v>
       </c>
       <c r="H40" s="18">
         <f>+D40/$B40</f>
-        <v>2.579359859183604</v>
+        <v>3.42344370512519</v>
       </c>
       <c r="I40" s="18">
         <f>+E40/$B40</f>
-        <v>0.44195001212354601</v>
-      </c>
-      <c r="K40" s="80">
-        <v>1.8856321828307002E-2</v>
-      </c>
-      <c r="L40" s="80">
-        <v>8.6830087745248793E-2</v>
-      </c>
-      <c r="M40" s="80">
-        <v>8.4460871513142702E-2</v>
-      </c>
-      <c r="N40" s="80">
-        <v>9.4961968222837298E-2</v>
-      </c>
+        <v>0.1736623214552562</v>
+      </c>
+      <c r="K40" s="80"/>
+      <c r="L40" s="80"/>
+      <c r="M40" s="80"/>
+      <c r="N40" s="80"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B41" s="73">
-        <f>-K39</f>
-        <v>-1.8856321828307002E-2</v>
-      </c>
-      <c r="C41" s="73">
-        <f t="shared" ref="C41:E41" si="9">-L39</f>
-        <v>-7.4986834877180303E-2</v>
-      </c>
-      <c r="D41" s="73">
-        <f t="shared" si="9"/>
-        <v>-0.114521497868232</v>
-      </c>
-      <c r="E41" s="73">
-        <f t="shared" si="9"/>
-        <v>-0.14262511117377299</v>
+      <c r="B41" s="73" t="str">
+        <f>IF(-K39=0,"",-K39)</f>
+        <v/>
+      </c>
+      <c r="C41" s="73" t="str">
+        <f t="shared" ref="C41:E41" si="10">IF(-L39=0,"",-L39)</f>
+        <v/>
+      </c>
+      <c r="D41" s="73" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="E41" s="73" t="str">
+        <f t="shared" si="10"/>
+        <v/>
       </c>
       <c r="F41" s="18"/>
       <c r="G41" s="18">
         <f>+C42/$B42</f>
-        <v>1.7865633911582248</v>
+        <v>2.262585613557953</v>
       </c>
       <c r="H41" s="18">
         <f>+D42/$B42</f>
-        <v>2.1717626166299819</v>
+        <v>2.5654818514854623</v>
       </c>
       <c r="I41" s="18">
         <f>+E42/$B42</f>
-        <v>0.23294604046745127</v>
-      </c>
-      <c r="K41" s="80">
-        <v>1.8856321828307002E-2</v>
-      </c>
-      <c r="L41" s="80">
-        <v>8.2373258308493402E-2</v>
-      </c>
-      <c r="M41" s="80">
-        <v>8.8718987609085004E-2</v>
-      </c>
-      <c r="N41" s="80">
-        <v>3.5278908100360003E-2</v>
-      </c>
+        <v>9.1339000944852186E-2</v>
+      </c>
+      <c r="K41" s="80"/>
+      <c r="L41" s="80"/>
+      <c r="M41" s="80"/>
+      <c r="N41" s="80"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>9</v>
       </c>
       <c r="B42" s="72">
-        <v>0.30002408033317401</v>
+        <f>+G46</f>
+        <v>0.26143821264262401</v>
       </c>
       <c r="C42" s="72">
-        <v>0.536012038389163</v>
+        <f t="shared" ref="C42:E42" si="11">+H46</f>
+        <v>0.591526338759506</v>
       </c>
       <c r="D42" s="72">
-        <v>0.65158108175637797</v>
+        <f t="shared" si="11"/>
+        <v>0.67071498981944899</v>
       </c>
       <c r="E42" s="72">
-        <v>6.9889421558501405E-2</v>
+        <f t="shared" si="11"/>
+        <v>2.3879505151585101E-2</v>
       </c>
       <c r="G42" s="18">
         <f>+C44/$B44</f>
-        <v>2.0941196035909679</v>
+        <v>2.8279023310241773</v>
       </c>
       <c r="H42" s="18">
         <f>+D44/$B44</f>
-        <v>1.8396516475591123</v>
+        <v>1.8466378672121815</v>
       </c>
       <c r="I42" s="18">
         <f>+E44/$B44</f>
-        <v>0.15281934113026216</v>
+        <v>9.1067511040164736E-2</v>
       </c>
       <c r="K42" s="75"/>
     </row>
     <row r="43" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="73">
-        <f>-K40</f>
-        <v>-1.8856321828307002E-2</v>
-      </c>
-      <c r="C43" s="73">
-        <f t="shared" ref="C43:E43" si="10">-L40</f>
-        <v>-8.6830087745248793E-2</v>
-      </c>
-      <c r="D43" s="73">
-        <f t="shared" si="10"/>
-        <v>-8.4460871513142702E-2</v>
-      </c>
-      <c r="E43" s="73">
-        <f t="shared" si="10"/>
-        <v>-9.4961968222837298E-2</v>
+      <c r="B43" s="73" t="str">
+        <f>IF(-K40=0,"",-K40)</f>
+        <v/>
+      </c>
+      <c r="C43" s="73" t="str">
+        <f t="shared" ref="C43:E43" si="12">IF(-L40=0,"",-L40)</f>
+        <v/>
+      </c>
+      <c r="D43" s="73" t="str">
+        <f t="shared" si="12"/>
+        <v/>
+      </c>
+      <c r="E43" s="73" t="str">
+        <f t="shared" si="12"/>
+        <v/>
       </c>
       <c r="F43" s="81"/>
       <c r="G43" s="82"/>
@@ -3316,16 +3277,20 @@
         <v>10</v>
       </c>
       <c r="B44" s="72">
-        <v>0.30002408033317401</v>
+        <f>+G47</f>
+        <v>0.26143821264262401</v>
       </c>
       <c r="C44" s="72">
-        <v>0.62828630817505104</v>
+        <f t="shared" ref="C44:E44" si="13">+H47</f>
+        <v>0.73932173095087095</v>
       </c>
       <c r="D44" s="72">
-        <v>0.55193979369233104</v>
+        <f t="shared" si="13"/>
+        <v>0.48278170340213999</v>
       </c>
       <c r="E44" s="72">
-        <v>4.5849482279728501E-2</v>
+        <f t="shared" si="13"/>
+        <v>2.38085273161531E-2</v>
       </c>
       <c r="F44" s="81"/>
       <c r="G44" s="81"/>
@@ -3336,50 +3301,50 @@
     </row>
     <row r="45" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="19"/>
-      <c r="B45" s="74">
-        <f t="array" ref="B45">-K41:N41</f>
-        <v>-1.8856321828307002E-2</v>
-      </c>
-      <c r="C45" s="74">
-        <f t="shared" ref="C45:E45" si="11">-H47</f>
-        <v>-8.8625088080741696E-2</v>
-      </c>
-      <c r="D45" s="74">
-        <f t="shared" si="11"/>
-        <v>-8.7677991056143698E-2</v>
-      </c>
-      <c r="E45" s="74">
-        <f t="shared" si="11"/>
-        <v>-7.5233432632621805E-2</v>
+      <c r="B45" s="74" t="str">
+        <f>IF(-K41=0,"",K41)</f>
+        <v/>
+      </c>
+      <c r="C45" s="74" t="str">
+        <f t="shared" ref="C45:E45" si="14">IF(-L41=0,"",L41)</f>
+        <v/>
+      </c>
+      <c r="D45" s="74" t="str">
+        <f t="shared" si="14"/>
+        <v/>
+      </c>
+      <c r="E45" s="74" t="str">
+        <f t="shared" si="14"/>
+        <v/>
       </c>
       <c r="F45" s="81"/>
       <c r="G45" s="83">
-        <v>3.27791808747964E-2</v>
+        <v>0.26143821264262401</v>
       </c>
       <c r="H45" s="83">
-        <v>7.5396741976460305E-2</v>
+        <v>0.37164357323102198</v>
       </c>
       <c r="I45" s="83">
-        <v>0.115293505002319</v>
+        <v>0.89501900335057205</v>
       </c>
       <c r="J45" s="80">
-        <v>0.14196233908585501</v>
+        <v>4.5401966924630999E-2</v>
       </c>
       <c r="K45" s="75"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="F46" s="81"/>
       <c r="G46" s="80">
-        <v>3.5902339137002803E-2</v>
+        <v>0.26143821264262401</v>
       </c>
       <c r="H46" s="80">
-        <v>8.7285450730600303E-2</v>
+        <v>0.591526338759506</v>
       </c>
       <c r="I46" s="80">
-        <v>8.3582228841739506E-2</v>
+        <v>0.67071498981944899</v>
       </c>
       <c r="J46" s="80">
-        <v>9.8175524348070906E-2</v>
+        <v>2.3879505151585101E-2</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.35">
@@ -3391,16 +3356,16 @@
       </c>
       <c r="F47" s="81"/>
       <c r="G47" s="80">
-        <v>3.5398027084865398E-2</v>
+        <v>0.26143821264262401</v>
       </c>
       <c r="H47" s="80">
-        <v>8.8625088080741696E-2</v>
+        <v>0.73932173095087095</v>
       </c>
       <c r="I47" s="80">
-        <v>8.7677991056143698E-2</v>
+        <v>0.48278170340213999</v>
       </c>
       <c r="J47" s="80">
-        <v>7.5233432632621805E-2</v>
+        <v>2.38085273161531E-2</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.35">
@@ -3436,20 +3401,20 @@
       <c r="E49" s="1"/>
     </row>
     <row r="51" spans="1:9" ht="18.5" hidden="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="99" t="s">
+      <c r="A51" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="B51" s="99"/>
-      <c r="C51" s="99"/>
-      <c r="D51" s="99"/>
-      <c r="E51" s="99"/>
+      <c r="B51" s="100"/>
+      <c r="C51" s="100"/>
+      <c r="D51" s="100"/>
+      <c r="E51" s="100"/>
     </row>
     <row r="52" spans="1:9" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G52" s="85" t="s">
+      <c r="G52" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="H52" s="85"/>
-      <c r="I52" s="85"/>
+      <c r="H52" s="86"/>
+      <c r="I52" s="86"/>
     </row>
     <row r="53" spans="1:9" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="10" t="s">
@@ -3494,15 +3459,15 @@
         <v>0.15027534446115601</v>
       </c>
       <c r="G54" s="18">
-        <f t="shared" ref="G54:G56" si="12">+C54/$B54</f>
+        <f t="shared" ref="G54:G56" si="15">+C54/$B54</f>
         <v>1.373671978812486</v>
       </c>
       <c r="H54" s="18">
-        <f t="shared" ref="H54:H56" si="13">+D54/$B54</f>
+        <f t="shared" ref="H54:H56" si="16">+D54/$B54</f>
         <v>2.882317701442024</v>
       </c>
       <c r="I54" s="18">
-        <f t="shared" ref="I54:I56" si="14">+E54/$B54</f>
+        <f t="shared" ref="I54:I56" si="17">+E54/$B54</f>
         <v>0.54826548178845746</v>
       </c>
     </row>
@@ -3523,15 +3488,15 @@
         <v>7.8971052048355805E-2</v>
       </c>
       <c r="G55" s="18">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>2.1206583692359722</v>
       </c>
       <c r="H55" s="18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>2.2750245955063209</v>
       </c>
       <c r="I55" s="18">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.28811846716361922</v>
       </c>
     </row>
@@ -3552,15 +3517,15 @@
         <v>0.13010063352593601</v>
       </c>
       <c r="G56" s="18">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>1.8654374748940057</v>
       </c>
       <c r="H56" s="18">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>2.2505536369075858</v>
       </c>
       <c r="I56" s="18">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>0.47465994356458474</v>
       </c>
     </row>
@@ -3643,7 +3608,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G40:G43 G45">
+  <conditionalFormatting sqref="G40:G43">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -3693,7 +3658,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H40:H43 H45">
+  <conditionalFormatting sqref="H40:H43">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -3743,7 +3708,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I40:I43 I45">
+  <conditionalFormatting sqref="I40:I43">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -3777,7 +3742,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3795,20 +3760,20 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="99" t="s">
+      <c r="A3" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="99"/>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
+      <c r="B3" s="100"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="G4" s="85" t="s">
+      <c r="G4" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
@@ -3988,8 +3953,8 @@
   </sheetPr>
   <dimension ref="A1:Q101"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E81" sqref="E81"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4129,10 +4094,10 @@
         <v>1.06E-5</v>
       </c>
       <c r="F10" s="28"/>
-      <c r="H10" s="100" t="s">
+      <c r="H10" s="101" t="s">
         <v>293</v>
       </c>
-      <c r="I10" s="100"/>
+      <c r="I10" s="101"/>
       <c r="L10" s="35"/>
     </row>
     <row r="11" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -4143,8 +4108,8 @@
       <c r="F11" s="28">
         <v>3.6207700000000002E-2</v>
       </c>
-      <c r="H11" s="100"/>
-      <c r="I11" s="100"/>
+      <c r="H11" s="101"/>
+      <c r="I11" s="101"/>
       <c r="L11" s="35"/>
       <c r="N11" s="35"/>
     </row>
@@ -4161,8 +4126,8 @@
       <c r="F12" s="28">
         <v>5.2985199999999999</v>
       </c>
-      <c r="H12" s="100"/>
-      <c r="I12" s="100"/>
+      <c r="H12" s="101"/>
+      <c r="I12" s="101"/>
       <c r="L12" s="35"/>
     </row>
     <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4178,8 +4143,8 @@
       <c r="F13" s="49">
         <v>30.137509999999999</v>
       </c>
-      <c r="H13" s="100"/>
-      <c r="I13" s="100"/>
+      <c r="H13" s="101"/>
+      <c r="I13" s="101"/>
       <c r="L13" s="35"/>
       <c r="N13" s="35"/>
     </row>
@@ -4347,8 +4312,8 @@
       <c r="E33" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="H33" s="89"/>
-      <c r="I33" s="89"/>
+      <c r="H33" s="90"/>
+      <c r="I33" s="90"/>
       <c r="L33" s="35"/>
     </row>
     <row r="34" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4356,10 +4321,10 @@
         <v>290</v>
       </c>
       <c r="O34" s="79"/>
-      <c r="P34" s="89" t="s">
+      <c r="P34" s="90" t="s">
         <v>280</v>
       </c>
-      <c r="Q34" s="89"/>
+      <c r="Q34" s="90"/>
     </row>
     <row r="35" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="10" t="s">
@@ -4489,10 +4454,10 @@
     <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="C40" s="9"/>
       <c r="F40" s="28"/>
-      <c r="H40" s="100" t="s">
+      <c r="H40" s="101" t="s">
         <v>293</v>
       </c>
-      <c r="I40" s="100"/>
+      <c r="I40" s="101"/>
       <c r="K40" t="s">
         <v>288</v>
       </c>
@@ -4510,8 +4475,8 @@
       <c r="F41" s="28">
         <v>1.365048</v>
       </c>
-      <c r="H41" s="100"/>
-      <c r="I41" s="100"/>
+      <c r="H41" s="101"/>
+      <c r="I41" s="101"/>
       <c r="K41" t="s">
         <v>289</v>
       </c>
@@ -4524,8 +4489,8 @@
       <c r="F42" s="28">
         <v>-0.3439432</v>
       </c>
-      <c r="H42" s="100"/>
-      <c r="I42" s="100"/>
+      <c r="H42" s="101"/>
+      <c r="I42" s="101"/>
     </row>
     <row r="43" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B43" s="35">
@@ -4540,8 +4505,8 @@
       <c r="F43" s="49">
         <v>13.51919</v>
       </c>
-      <c r="H43" s="100"/>
-      <c r="I43" s="100"/>
+      <c r="H43" s="101"/>
+      <c r="I43" s="101"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B44" s="35">
@@ -5324,10 +5289,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10ED2790-90CA-437E-8990-4813411B73C2}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21:N35"/>
+    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5336,7 +5301,7 @@
     <col min="3" max="6" width="13.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>140</v>
       </c>
@@ -5344,7 +5309,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
@@ -5361,10 +5326,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="35"/>
     </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="40"/>
       <c r="C4" s="10" t="s">
         <v>3</v>
@@ -5379,260 +5344,342 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B5" s="35">
         <v>0.01</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C5" s="9">
+        <v>-15.10528</v>
+      </c>
+      <c r="D5" s="9">
+        <v>-15.579129999999999</v>
+      </c>
+      <c r="E5" s="9">
+        <v>-15.55288</v>
+      </c>
+      <c r="F5" s="9">
+        <v>-14.47852</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B6" s="35">
         <v>0.05</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C6" s="9">
+        <v>-1.4926399999999999E-2</v>
+      </c>
+      <c r="D6" s="9">
+        <v>-1.63663E-2</v>
+      </c>
+      <c r="E6" s="9">
+        <v>-1.7490700000000001E-2</v>
+      </c>
+      <c r="F6" s="9">
+        <v>-1.8323900000000001E-2</v>
+      </c>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B7" s="35">
         <v>0.1</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C7" s="9">
+        <v>-8.7606000000000003E-3</v>
+      </c>
+      <c r="D7" s="9">
+        <v>-8.7720000000000003E-3</v>
+      </c>
+      <c r="E7" s="9">
+        <v>-8.6779000000000005E-3</v>
+      </c>
+      <c r="F7" s="9">
+        <v>-8.4244999999999997E-3</v>
+      </c>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B8" s="35">
         <v>0.25</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C8" s="9">
+        <v>-3.3000999999999998E-3</v>
+      </c>
+      <c r="D8" s="9">
+        <v>-3.0918E-3</v>
+      </c>
+      <c r="E8" s="9">
+        <v>-2.6830999999999999E-3</v>
+      </c>
+      <c r="F8" s="9">
+        <v>-3.5279999999999999E-3</v>
+      </c>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B10" s="35">
         <v>0.5</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C10" s="9">
+        <v>1.058E-4</v>
+      </c>
+      <c r="D10" s="9">
+        <v>4.9100000000000004E-6</v>
+      </c>
+      <c r="E10" s="9">
+        <v>-1.73E-5</v>
+      </c>
+      <c r="F10" s="9">
+        <v>-1.8870000000000001E-4</v>
+      </c>
+      <c r="J10" s="35"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="85"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B12" s="35">
         <v>0.75</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C12" s="9">
+        <v>2.5374E-3</v>
+      </c>
+      <c r="D12" s="9">
+        <v>2.9001000000000001E-3</v>
+      </c>
+      <c r="E12" s="9">
+        <v>2.8260999999999998E-3</v>
+      </c>
+      <c r="F12" s="9">
+        <v>2.5098999999999998E-3</v>
+      </c>
+      <c r="J12" s="35"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B13" s="35">
         <v>0.9</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C13" s="9">
+        <v>8.8976999999999997E-3</v>
+      </c>
+      <c r="D13" s="9">
+        <v>8.5959999999999995E-3</v>
+      </c>
+      <c r="E13" s="9">
+        <v>7.9916999999999992E-3</v>
+      </c>
+      <c r="F13" s="9">
+        <v>7.3561E-3</v>
+      </c>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B14" s="35">
         <v>0.95</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C14" s="9">
+        <v>4.6813899999999999E-2</v>
+      </c>
+      <c r="D14" s="9">
+        <v>5.4863200000000001E-2</v>
+      </c>
+      <c r="E14" s="9">
+        <v>5.4990700000000003E-2</v>
+      </c>
+      <c r="F14" s="9">
+        <v>3.78941E-2</v>
+      </c>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+    </row>
+    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="45">
         <v>0.99</v>
       </c>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="46"/>
-    </row>
-    <row r="16" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
+      <c r="C15" s="46">
+        <v>7.06684</v>
+      </c>
+      <c r="D15" s="46">
+        <v>6.6164230000000002</v>
+      </c>
+      <c r="E15" s="46">
+        <v>7.7228779999999997</v>
+      </c>
+      <c r="F15" s="46">
+        <v>6.145689</v>
+      </c>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+    </row>
+    <row r="16" spans="1:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="84">
+        <v>0.45749050000000002</v>
+      </c>
+      <c r="D17" s="84">
+        <v>0.45225169999999998</v>
+      </c>
+      <c r="E17" s="84">
+        <v>0.45868720000000002</v>
+      </c>
+      <c r="F17" s="84">
+        <v>-0.11019139999999999</v>
+      </c>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+    </row>
+    <row r="18" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="49">
+        <v>7.9427960000000004</v>
+      </c>
+      <c r="D18" s="49">
+        <v>7.9220100000000002</v>
+      </c>
+      <c r="E18" s="49">
+        <v>7.9490109999999996</v>
+      </c>
+      <c r="F18" s="49">
+        <v>7.0228719999999996</v>
+      </c>
+      <c r="I18" s="35"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I19" s="35"/>
+    </row>
+    <row r="20" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>296</v>
+      </c>
+      <c r="C20" s="28">
+        <v>744</v>
+      </c>
+      <c r="I20" s="35"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B23" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C23" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D23" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E23" s="21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B20" s="35"/>
-    </row>
-    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="40"/>
-      <c r="C21" s="11" t="s">
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="35"/>
+    </row>
+    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="40"/>
+      <c r="C25" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D25" s="11" t="s">
         <v>295</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E25" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F25" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I21" s="35"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B22" s="35">
+      <c r="I25" s="35"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B26" s="35">
         <v>0.01</v>
       </c>
-      <c r="C22" s="28">
+      <c r="C26" s="28">
         <v>-28.530819999999999</v>
       </c>
-      <c r="D22" s="28">
+      <c r="D26" s="28">
         <v>-28.695879999999999</v>
       </c>
-      <c r="E22" s="28">
+      <c r="E26" s="28">
         <v>-28.70872</v>
       </c>
-      <c r="F22" s="28">
+      <c r="F26" s="28">
         <v>-28.650200000000002</v>
       </c>
-      <c r="H22" s="35"/>
-      <c r="I22" s="48"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B23" s="35">
-        <v>0.05</v>
-      </c>
-      <c r="C23" s="28">
-        <v>-11.735849999999999</v>
-      </c>
-      <c r="D23" s="28">
-        <v>-9.3291360000000001</v>
-      </c>
-      <c r="E23" s="28">
-        <v>-9.1838979999999992</v>
-      </c>
-      <c r="F23" s="28">
-        <v>-10.03772</v>
-      </c>
-      <c r="H23" s="35"/>
-      <c r="I23" s="48"/>
-      <c r="K23" s="35"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B24" s="35">
-        <v>0.1</v>
-      </c>
-      <c r="C24" s="28">
-        <v>-6.3795130000000002</v>
-      </c>
-      <c r="D24" s="28">
-        <v>-6.5917760000000003</v>
-      </c>
-      <c r="E24" s="28">
-        <v>-5.859515</v>
-      </c>
-      <c r="F24" s="28">
-        <v>-6.8069100000000002</v>
-      </c>
-      <c r="H24" s="35"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="35"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B25" s="35">
-        <v>0.25</v>
-      </c>
-      <c r="C25" s="28">
-        <v>-1.7284900000000001</v>
-      </c>
-      <c r="D25" s="28">
-        <v>-1.915889</v>
-      </c>
-      <c r="E25" s="28">
-        <v>-2.0371790000000001</v>
-      </c>
-      <c r="F25" s="28">
-        <v>-2.0360320000000001</v>
-      </c>
-      <c r="H25" s="35"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="35"/>
-      <c r="K25" s="35"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
       <c r="H26" s="35"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="35"/>
-      <c r="K26" s="35"/>
+      <c r="I26" s="48"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B27" s="35">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="C27" s="28">
-        <v>1.73343E-2</v>
+        <v>-11.735849999999999</v>
       </c>
       <c r="D27" s="28">
-        <v>5.6809999999999999E-4</v>
+        <v>-9.3291360000000001</v>
       </c>
       <c r="E27" s="28">
-        <v>2.42992E-2</v>
+        <v>-9.1838979999999992</v>
       </c>
       <c r="F27" s="28">
-        <v>1.11273E-2</v>
+        <v>-10.03772</v>
       </c>
       <c r="H27" s="35"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="35"/>
+      <c r="I27" s="48"/>
+      <c r="K27" s="35"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
+      <c r="B28" s="35">
+        <v>0.1</v>
+      </c>
+      <c r="C28" s="28">
+        <v>-6.3795130000000002</v>
+      </c>
+      <c r="D28" s="28">
+        <v>-6.5917760000000003</v>
+      </c>
+      <c r="E28" s="28">
+        <v>-5.859515</v>
+      </c>
+      <c r="F28" s="28">
+        <v>-6.8069100000000002</v>
+      </c>
       <c r="H28" s="35"/>
       <c r="I28" s="28"/>
       <c r="J28" s="35"/>
@@ -5640,140 +5687,201 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B29" s="35">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="C29" s="28">
-        <v>1.7843549999999999</v>
+        <v>-1.7284900000000001</v>
       </c>
       <c r="D29" s="28">
-        <v>1.6439379999999999</v>
+        <v>-1.915889</v>
       </c>
       <c r="E29" s="28">
-        <v>1.7495000000000001</v>
+        <v>-2.0371790000000001</v>
       </c>
       <c r="F29" s="28">
-        <v>1.905146</v>
+        <v>-2.0360320000000001</v>
       </c>
       <c r="H29" s="35"/>
       <c r="I29" s="28"/>
       <c r="J29" s="35"/>
+      <c r="K29" s="35"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B30" s="35">
-        <v>0.9</v>
-      </c>
-      <c r="C30" s="28">
-        <v>5.8339160000000003</v>
-      </c>
-      <c r="D30" s="28">
-        <v>6.2187260000000002</v>
-      </c>
-      <c r="E30" s="28">
-        <v>5.9841689999999996</v>
-      </c>
-      <c r="F30" s="28">
-        <v>5.7457029999999998</v>
-      </c>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
       <c r="H30" s="35"/>
       <c r="I30" s="28"/>
+      <c r="J30" s="35"/>
       <c r="K30" s="35"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B31" s="35">
-        <v>0.95</v>
+        <v>0.5</v>
       </c>
       <c r="C31" s="28">
-        <v>8.2809310000000007</v>
+        <v>1.73343E-2</v>
       </c>
       <c r="D31" s="28">
-        <v>8.7441630000000004</v>
+        <v>5.6809999999999999E-4</v>
       </c>
       <c r="E31" s="28">
-        <v>9.275582</v>
+        <v>2.42992E-2</v>
       </c>
       <c r="F31" s="28">
-        <v>9.2394499999999997</v>
+        <v>1.11273E-2</v>
       </c>
       <c r="H31" s="35"/>
-      <c r="I31" s="35"/>
+      <c r="I31" s="28"/>
       <c r="J31" s="35"/>
-      <c r="K31" s="35"/>
-    </row>
-    <row r="32" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="45">
-        <v>0.99</v>
-      </c>
-      <c r="C32" s="68">
-        <v>24.982859999999999</v>
-      </c>
-      <c r="D32" s="68">
-        <v>24.365179999999999</v>
-      </c>
-      <c r="E32" s="68">
-        <v>24.45382</v>
-      </c>
-      <c r="F32" s="68">
-        <v>24.421749999999999</v>
-      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
       <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
+      <c r="I32" s="28"/>
       <c r="J32" s="35"/>
       <c r="K32" s="35"/>
     </row>
-    <row r="33" spans="2:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B33" s="35">
+        <v>0.75</v>
+      </c>
+      <c r="C33" s="28">
+        <v>1.7843549999999999</v>
+      </c>
+      <c r="D33" s="28">
+        <v>1.6439379999999999</v>
+      </c>
+      <c r="E33" s="28">
+        <v>1.7495000000000001</v>
+      </c>
+      <c r="F33" s="28">
+        <v>1.905146</v>
+      </c>
       <c r="H33" s="35"/>
-      <c r="I33" s="35"/>
+      <c r="I33" s="28"/>
       <c r="J33" s="35"/>
-      <c r="K33" s="35"/>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="35">
+        <v>0.9</v>
+      </c>
+      <c r="C34" s="28">
+        <v>5.8339160000000003</v>
+      </c>
+      <c r="D34" s="28">
+        <v>6.2187260000000002</v>
+      </c>
+      <c r="E34" s="28">
+        <v>5.9841689999999996</v>
+      </c>
+      <c r="F34" s="28">
+        <v>5.7457029999999998</v>
+      </c>
+      <c r="H34" s="35"/>
+      <c r="I34" s="28"/>
+      <c r="K34" s="35"/>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B35" s="35">
+        <v>0.95</v>
+      </c>
+      <c r="C35" s="28">
+        <v>8.2809310000000007</v>
+      </c>
+      <c r="D35" s="28">
+        <v>8.7441630000000004</v>
+      </c>
+      <c r="E35" s="28">
+        <v>9.275582</v>
+      </c>
+      <c r="F35" s="28">
+        <v>9.2394499999999997</v>
+      </c>
+      <c r="H35" s="35"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="35"/>
+    </row>
+    <row r="36" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B36" s="45">
+        <v>0.99</v>
+      </c>
+      <c r="C36" s="68">
+        <v>24.982859999999999</v>
+      </c>
+      <c r="D36" s="68">
+        <v>24.365179999999999</v>
+      </c>
+      <c r="E36" s="68">
+        <v>24.45382</v>
+      </c>
+      <c r="F36" s="68">
+        <v>24.421749999999999</v>
+      </c>
+      <c r="H36" s="35"/>
+      <c r="I36" s="35"/>
+      <c r="J36" s="35"/>
+      <c r="K36" s="35"/>
+    </row>
+    <row r="37" spans="2:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
+      <c r="K37" s="35"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B38" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="84">
+      <c r="C38" s="84">
         <v>-0.24654670000000001</v>
       </c>
-      <c r="D34" s="84">
+      <c r="D38" s="84">
         <v>-0.1275568</v>
       </c>
-      <c r="E34" s="84">
+      <c r="E38" s="84">
         <v>-9.1481199999999999E-2</v>
       </c>
-      <c r="F34" s="84">
+      <c r="F38" s="84">
         <v>-0.11019139999999999</v>
       </c>
-      <c r="J34" s="35"/>
-    </row>
-    <row r="35" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="19" t="s">
+      <c r="J38" s="35"/>
+    </row>
+    <row r="39" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B39" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="49">
+      <c r="C39" s="49">
         <v>7.2521839999999997</v>
       </c>
-      <c r="D35" s="49">
+      <c r="D39" s="49">
         <v>6.9003690000000004</v>
       </c>
-      <c r="E35" s="49">
+      <c r="E39" s="49">
         <v>7.0136580000000004</v>
       </c>
-      <c r="F35" s="49">
+      <c r="F39" s="49">
         <v>7.0228719999999996</v>
       </c>
-      <c r="J35" s="35"/>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="J36" s="35"/>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B37" t="s">
+      <c r="J39" s="35"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="J40" s="35"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
         <v>296</v>
       </c>
-      <c r="C37" s="28">
+      <c r="C41" s="28">
         <v>744</v>
       </c>
     </row>
@@ -5817,12 +5925,12 @@
       <c r="B3" s="62"/>
     </row>
     <row r="4" spans="1:4" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="91" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="90"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
     </row>
     <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6386,66 +6494,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B1" s="86" t="s">
+      <c r="B1" s="87" t="s">
         <v>215</v>
       </c>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
       <c r="G1" s="54"/>
-      <c r="H1" s="86" t="s">
+      <c r="H1" s="87" t="s">
         <v>248</v>
       </c>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="N1" s="86" t="s">
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="N1" s="87" t="s">
         <v>212</v>
       </c>
-      <c r="O1" s="86"/>
-      <c r="P1" s="86"/>
-      <c r="Q1" s="86"/>
-      <c r="R1" s="86"/>
-      <c r="T1" s="86" t="s">
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="87"/>
+      <c r="R1" s="87"/>
+      <c r="T1" s="87" t="s">
         <v>213</v>
       </c>
-      <c r="U1" s="86"/>
-      <c r="V1" s="86"/>
-      <c r="W1" s="86"/>
-      <c r="X1" s="86"/>
+      <c r="U1" s="87"/>
+      <c r="V1" s="87"/>
+      <c r="W1" s="87"/>
+      <c r="X1" s="87"/>
     </row>
     <row r="2" spans="2:27" x14ac:dyDescent="0.35">
-      <c r="B2" s="87" t="s">
+      <c r="B2" s="88" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
       <c r="G2" s="54"/>
-      <c r="H2" s="87" t="s">
+      <c r="H2" s="88" t="s">
         <v>214</v>
       </c>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="87"/>
-      <c r="N2" s="87" t="s">
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="N2" s="88" t="s">
         <v>214</v>
       </c>
-      <c r="O2" s="87"/>
-      <c r="P2" s="87"/>
-      <c r="Q2" s="87"/>
-      <c r="R2" s="87"/>
-      <c r="T2" s="87" t="s">
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="88"/>
+      <c r="T2" s="88" t="s">
         <v>214</v>
       </c>
-      <c r="U2" s="88"/>
-      <c r="V2" s="88"/>
-      <c r="W2" s="88"/>
-      <c r="X2" s="88"/>
+      <c r="U2" s="89"/>
+      <c r="V2" s="89"/>
+      <c r="W2" s="89"/>
+      <c r="X2" s="89"/>
     </row>
     <row r="3" spans="2:27" hidden="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4"/>
@@ -7480,10 +7588,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="90" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="89"/>
+      <c r="C2" s="90"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
@@ -8018,13 +8126,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="90"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
       <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -8138,12 +8246,12 @@
       <c r="E8" s="9"/>
     </row>
     <row r="10" spans="1:10" ht="46" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A10" s="91" t="s">
+      <c r="A10" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="91"/>
-      <c r="C10" s="91"/>
-      <c r="D10" s="91"/>
+      <c r="B10" s="92"/>
+      <c r="C10" s="92"/>
+      <c r="D10" s="92"/>
     </row>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="13"/>
@@ -8442,12 +8550,12 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A37" s="91" t="s">
+      <c r="A37" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="B37" s="91"/>
-      <c r="C37" s="91"/>
-      <c r="D37" s="91"/>
+      <c r="B37" s="92"/>
+      <c r="C37" s="92"/>
+      <c r="D37" s="92"/>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="13"/>
@@ -8781,13 +8889,13 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="92" t="s">
+      <c r="A3" s="93" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
@@ -9025,13 +9133,13 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="93" t="s">
+      <c r="A21" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="93"/>
-      <c r="C21" s="93"/>
-      <c r="D21" s="93"/>
-      <c r="E21" s="93"/>
+      <c r="B21" s="94"/>
+      <c r="C21" s="94"/>
+      <c r="D21" s="94"/>
+      <c r="E21" s="94"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="50"/>
@@ -9059,13 +9167,13 @@
       <c r="E24" s="50"/>
     </row>
     <row r="25" spans="1:5" ht="33.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="92" t="s">
+      <c r="A25" s="93" t="s">
         <v>128</v>
       </c>
-      <c r="B25" s="92"/>
-      <c r="C25" s="92"/>
-      <c r="D25" s="92"/>
-      <c r="E25" s="92"/>
+      <c r="B25" s="93"/>
+      <c r="C25" s="93"/>
+      <c r="D25" s="93"/>
+      <c r="E25" s="93"/>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1"/>
@@ -9327,13 +9435,13 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="93" t="s">
+      <c r="A43" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="93"/>
-      <c r="C43" s="93"/>
-      <c r="D43" s="93"/>
-      <c r="E43" s="93"/>
+      <c r="B43" s="94"/>
+      <c r="C43" s="94"/>
+      <c r="D43" s="94"/>
+      <c r="E43" s="94"/>
     </row>
     <row r="45" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
@@ -9701,36 +9809,36 @@
       <c r="AB2"/>
     </row>
     <row r="3" spans="1:29" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="94" t="s">
+      <c r="A3" s="95" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="94"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="94"/>
-      <c r="J3" s="94"/>
-      <c r="K3" s="94"/>
-      <c r="L3" s="94"/>
-      <c r="M3" s="94"/>
-      <c r="N3" s="94"/>
-      <c r="O3" s="94"/>
-      <c r="P3" s="94"/>
-      <c r="Q3" s="94"/>
-      <c r="R3" s="94"/>
-      <c r="S3" s="94"/>
-      <c r="T3" s="94"/>
-      <c r="U3" s="94"/>
-      <c r="V3" s="94"/>
-      <c r="W3" s="94"/>
-      <c r="X3" s="94"/>
-      <c r="Y3" s="94"/>
-      <c r="Z3" s="94"/>
-      <c r="AA3" s="94"/>
-      <c r="AB3" s="94"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="95"/>
+      <c r="O3" s="95"/>
+      <c r="P3" s="95"/>
+      <c r="Q3" s="95"/>
+      <c r="R3" s="95"/>
+      <c r="S3" s="95"/>
+      <c r="T3" s="95"/>
+      <c r="U3" s="95"/>
+      <c r="V3" s="95"/>
+      <c r="W3" s="95"/>
+      <c r="X3" s="95"/>
+      <c r="Y3" s="95"/>
+      <c r="Z3" s="95"/>
+      <c r="AA3" s="95"/>
+      <c r="AB3" s="95"/>
       <c r="AC3" s="32"/>
     </row>
     <row r="4" spans="1:29" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -10214,35 +10322,35 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="B4" s="97" t="s">
+      <c r="B4" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="97"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="98" t="s">
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98"/>
-      <c r="K4" s="95" t="s">
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
+      <c r="H4" s="99"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="99"/>
+      <c r="K4" s="96" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="95"/>
-      <c r="M4" s="95"/>
-      <c r="N4" s="95"/>
-      <c r="O4" s="96" t="s">
+      <c r="L4" s="96"/>
+      <c r="M4" s="96"/>
+      <c r="N4" s="96"/>
+      <c r="O4" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="96"/>
-      <c r="Q4" s="96"/>
-      <c r="R4" s="96"/>
-      <c r="S4" s="96"/>
-      <c r="T4" s="96"/>
-      <c r="U4" s="96"/>
-      <c r="V4" s="96"/>
+      <c r="P4" s="97"/>
+      <c r="Q4" s="97"/>
+      <c r="R4" s="97"/>
+      <c r="S4" s="97"/>
+      <c r="T4" s="97"/>
+      <c r="U4" s="97"/>
+      <c r="V4" s="97"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B5" s="36" t="s">

</xml_diff>